<commit_message>
Week 5 without writeup
</commit_message>
<xml_diff>
--- a/RiskRegister.xlsx
+++ b/RiskRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffaa5fcd33f076d1/Documents/GitHub/Project_ECEN3753_HarkonnenPong_Week1/Project_ECEN3753_HarkonnenPong_Tommy_Ramirez/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{02B1A892-D90B-44EF-934C-78F32540FE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{02B1A892-D90B-44EF-934C-78F32540FE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F97A59F-511E-4CA4-A47C-857DF4A0DC4A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -83,12 +83,6 @@
     <t>Changes in PWM can't be recognized/decoded</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Use own judgement for which PWMs are distinct enough</t>
-  </si>
-  <si>
     <t>My slider is sticking after some time operating</t>
   </si>
   <si>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>New includes seemingly made the problem disappear</t>
+  </si>
+  <si>
+    <t>Differences have been made very noticable</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1523,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1618,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1641,17 +1638,19 @@
       <c r="E4" s="2">
         <v>44637</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1667,13 +1666,13 @@
         <v>44631</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>